<commit_message>
Table is now updated with new work order additions
</commit_message>
<xml_diff>
--- a/src/Files/WorkOrders/185A 110V FORMULATED 1-4-2017.xlsx
+++ b/src/Files/WorkOrders/185A 110V FORMULATED 1-4-2017.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\eclipse-workspace\BURIN_V2\src\Files\WorkOrders\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="150" windowWidth="8700" windowHeight="10725"/>
+    <workbookView xWindow="1440" yWindow="150" windowWidth="8700" windowHeight="10728"/>
   </bookViews>
   <sheets>
     <sheet name="185-A WO " sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="133">
   <si>
     <t>BEAHMDESIGNS</t>
   </si>
@@ -407,6 +412,12 @@
   </si>
   <si>
     <t>DO NOT KIT - THESE ARE HOA'S FLOOR STOCK</t>
+  </si>
+  <si>
+    <t>START</t>
+  </si>
+  <si>
+    <t>END</t>
   </si>
 </sst>
 </file>
@@ -693,6 +704,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -740,7 +754,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -775,7 +789,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -987,28 +1001,28 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="4.27734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="5.71875" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="8" width="29.71875" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="11" max="12" width="10.71875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A1" s="43" t="s">
         <v>112</v>
       </c>
@@ -1028,7 +1042,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="14" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="14" customFormat="1" ht="14.1" x14ac:dyDescent="0.5">
       <c r="B3" s="16"/>
       <c r="C3" s="17" t="s">
         <v>114</v>
@@ -1069,7 +1083,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="42" t="s">
         <v>129</v>
       </c>
@@ -1083,7 +1097,7 @@
       <c r="I4" s="13"/>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" spans="1:13" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1095,80 +1109,61 @@
       <c r="I5" s="1"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="34" t="s">
+      <c r="B7" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D7" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E7" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G7" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I7" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row r="8" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="7">
         <v>5200</v>
-      </c>
-      <c r="B7" s="7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <f>SUM(B7*D3)</f>
-        <v>3</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K7" s="21">
-        <v>24.52</v>
-      </c>
-      <c r="L7" s="21">
-        <f t="shared" ref="L7:L20" si="0">K7*C7</f>
-        <v>73.56</v>
-      </c>
-      <c r="M7" s="23"/>
-    </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>5202</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
@@ -1179,31 +1174,29 @@
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
-      <c r="F8" s="6" t="s">
-        <v>90</v>
+      <c r="F8" s="24" t="s">
+        <v>97</v>
       </c>
       <c r="G8" s="24"/>
-      <c r="H8" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="H8" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="24"/>
       <c r="J8" s="6" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="K8" s="21">
-        <v>99</v>
+        <v>24.52</v>
       </c>
       <c r="L8" s="21">
-        <f t="shared" si="0"/>
-        <v>297</v>
+        <f t="shared" ref="L8:L21" si="0">K8*C8</f>
+        <v>73.56</v>
       </c>
       <c r="M8" s="23"/>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7">
-        <v>5349</v>
+        <v>5202</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
@@ -1214,31 +1207,31 @@
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
-      <c r="F9" s="24" t="s">
-        <v>85</v>
+      <c r="F9" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="G9" s="24"/>
-      <c r="H9" s="24" t="s">
-        <v>86</v>
+      <c r="H9" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K9" s="21">
-        <v>286.66000000000003</v>
+        <v>99</v>
       </c>
       <c r="L9" s="21">
         <f t="shared" si="0"/>
-        <v>859.98</v>
+        <v>297</v>
       </c>
       <c r="M9" s="23"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="7">
-        <v>5352</v>
+        <v>5349</v>
       </c>
       <c r="B10" s="7">
         <v>1</v>
@@ -1250,11 +1243,11 @@
       <c r="D10" s="24"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>50</v>
@@ -1263,17 +1256,17 @@
         <v>51</v>
       </c>
       <c r="K10" s="21">
-        <v>252.8</v>
+        <v>286.66000000000003</v>
       </c>
       <c r="L10" s="21">
         <f t="shared" si="0"/>
-        <v>758.40000000000009</v>
+        <v>859.98</v>
       </c>
       <c r="M10" s="23"/>
     </row>
-    <row r="11" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="7">
-        <v>6244</v>
+        <v>5352</v>
       </c>
       <c r="B11" s="7">
         <v>1</v>
@@ -1284,29 +1277,31 @@
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="F11" s="24" t="s">
+        <v>127</v>
+      </c>
       <c r="G11" s="24"/>
-      <c r="H11" s="6" t="s">
-        <v>63</v>
+      <c r="H11" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>119</v>
+        <v>50</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="K11" s="21">
-        <v>6.13</v>
+        <v>252.8</v>
       </c>
       <c r="L11" s="21">
         <f t="shared" si="0"/>
-        <v>18.39</v>
+        <v>758.40000000000009</v>
       </c>
       <c r="M11" s="23"/>
     </row>
-    <row r="12" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="7">
-        <v>6245</v>
+        <v>6244</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
@@ -1320,92 +1315,92 @@
       <c r="F12" s="24"/>
       <c r="G12" s="24"/>
       <c r="H12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K12" s="21">
-        <v>11.25</v>
+        <v>6.13</v>
       </c>
       <c r="L12" s="21">
         <f t="shared" si="0"/>
-        <v>33.75</v>
+        <v>18.39</v>
       </c>
       <c r="M12" s="23"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="7">
-        <v>6306</v>
+        <v>6245</v>
       </c>
       <c r="B13" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="7">
         <f>SUM(B13*D3)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D13" s="24"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
-      <c r="H13" s="24" t="s">
-        <v>62</v>
+      <c r="H13" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>119</v>
+      <c r="J13" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="K13" s="21">
-        <v>7</v>
+        <v>11.25</v>
       </c>
       <c r="L13" s="21">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>33.75</v>
       </c>
       <c r="M13" s="23"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7">
-        <v>6307</v>
+        <v>6306</v>
       </c>
       <c r="B14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="7">
         <f>SUM(B14*D3)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
       <c r="H14" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="K14" s="21">
-        <v>21.95</v>
+        <v>7</v>
       </c>
       <c r="L14" s="21">
         <f t="shared" si="0"/>
-        <v>65.849999999999994</v>
+        <v>42</v>
       </c>
       <c r="M14" s="23"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="7">
-        <v>6308</v>
+        <v>6307</v>
       </c>
       <c r="B15" s="7">
         <v>1</v>
@@ -1419,26 +1414,26 @@
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
       <c r="H15" s="24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="K15" s="21">
-        <v>12.5</v>
+        <v>21.95</v>
       </c>
       <c r="L15" s="21">
         <f t="shared" si="0"/>
-        <v>37.5</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="M15" s="23"/>
     </row>
-    <row r="16" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="32">
-        <v>6431</v>
+    <row r="16" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="7">
+        <v>6308</v>
       </c>
       <c r="B16" s="7">
         <v>1</v>
@@ -1449,10 +1444,10 @@
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="24"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="24"/>
       <c r="G16" s="24"/>
-      <c r="H16" s="6" t="s">
-        <v>101</v>
+      <c r="H16" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>59</v>
@@ -1461,83 +1456,83 @@
         <v>59</v>
       </c>
       <c r="K16" s="21">
-        <v>13.85</v>
+        <v>12.5</v>
       </c>
       <c r="L16" s="21">
         <f t="shared" si="0"/>
-        <v>41.55</v>
-      </c>
-      <c r="M16" s="28"/>
-    </row>
-    <row r="17" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>37.5</v>
+      </c>
+      <c r="M16" s="23"/>
+    </row>
+    <row r="17" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="32">
-        <v>6434</v>
+        <v>6431</v>
       </c>
       <c r="B17" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="7">
         <f>SUM(B17*D3)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="24"/>
       <c r="F17" s="6"/>
       <c r="G17" s="24"/>
       <c r="H17" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="K17" s="21">
-        <v>8.74</v>
+        <v>13.85</v>
       </c>
       <c r="L17" s="21">
         <f t="shared" si="0"/>
-        <v>52.44</v>
-      </c>
-      <c r="M17" s="23"/>
-    </row>
-    <row r="18" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>6466</v>
+        <v>41.55</v>
+      </c>
+      <c r="M17" s="28"/>
+    </row>
+    <row r="18" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="32">
+        <v>6434</v>
       </c>
       <c r="B18" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" s="7">
         <f>SUM(B18*D3)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="6">
-        <v>2860108655</v>
-      </c>
+      <c r="F18" s="6"/>
       <c r="G18" s="24"/>
       <c r="H18" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I18" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="J18" s="6" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="K18" s="21">
-        <v>7.32</v>
+        <v>8.74</v>
       </c>
       <c r="L18" s="21">
         <f t="shared" si="0"/>
-        <v>21.96</v>
+        <v>52.44</v>
       </c>
       <c r="M18" s="23"/>
     </row>
-    <row r="19" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="32">
-        <v>6543</v>
+    <row r="19" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="7">
+        <v>6466</v>
       </c>
       <c r="B19" s="7">
         <v>1</v>
@@ -1548,29 +1543,29 @@
       </c>
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="6"/>
+      <c r="F19" s="6">
+        <v>2860108655</v>
+      </c>
       <c r="G19" s="24"/>
       <c r="H19" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>59</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="I19" s="6"/>
       <c r="J19" s="6" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="K19" s="21">
-        <v>22.5</v>
+        <v>7.32</v>
       </c>
       <c r="L19" s="21">
         <f t="shared" si="0"/>
-        <v>67.5</v>
+        <v>21.96</v>
       </c>
       <c r="M19" s="23"/>
     </row>
-    <row r="20" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="32">
-        <v>6588</v>
+        <v>6543</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
@@ -1584,7 +1579,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="24"/>
       <c r="H20" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I20" s="6" t="s">
         <v>59</v>
@@ -1593,72 +1588,76 @@
         <v>59</v>
       </c>
       <c r="K20" s="21">
-        <v>39</v>
+        <v>22.5</v>
       </c>
       <c r="L20" s="21">
         <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="M20" s="23"/>
+    </row>
+    <row r="21" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="32">
+        <v>6588</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <f>SUM(B21*D3)</f>
+        <v>3</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="21">
+        <v>39</v>
+      </c>
+      <c r="L21" s="21">
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
-      <c r="M20" s="23"/>
-    </row>
-    <row r="21" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
+      <c r="M21" s="23"/>
+    </row>
+    <row r="22" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
+    <row r="23" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="7">
         <v>5004</v>
-      </c>
-      <c r="B23" s="7">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="K23" s="21">
-        <v>25.38</v>
-      </c>
-      <c r="L23" s="21">
-        <f t="shared" ref="L23:L54" si="1">K23*C23</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="23"/>
-    </row>
-    <row r="24" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>5008</v>
       </c>
       <c r="B24" s="7">
         <v>1</v>
@@ -1666,29 +1665,31 @@
       <c r="C24" s="7"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="24" t="s">
-        <v>82</v>
+      <c r="F24" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="G24" s="24"/>
-      <c r="H24" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="24"/>
+      <c r="H24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="J24" s="6" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="K24" s="21">
-        <v>3.64</v>
+        <v>25.38</v>
       </c>
       <c r="L24" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="L24:L55" si="1">K24*C24</f>
         <v>0</v>
       </c>
       <c r="M24" s="23"/>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="7">
-        <v>5012</v>
+        <v>5008</v>
       </c>
       <c r="B25" s="7">
         <v>1</v>
@@ -1696,19 +1697,19 @@
       <c r="C25" s="7"/>
       <c r="D25" s="24"/>
       <c r="E25" s="24"/>
-      <c r="F25" s="6">
-        <v>2860124541</v>
+      <c r="F25" s="24" t="s">
+        <v>82</v>
       </c>
       <c r="G25" s="24"/>
-      <c r="H25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I25" s="6"/>
+      <c r="H25" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I25" s="24"/>
       <c r="J25" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K25" s="21">
-        <v>10.06</v>
+        <v>3.64</v>
       </c>
       <c r="L25" s="21">
         <f t="shared" si="1"/>
@@ -1716,29 +1717,29 @@
       </c>
       <c r="M25" s="23"/>
     </row>
-    <row r="26" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="7">
-        <v>5015</v>
+        <v>5012</v>
       </c>
       <c r="B26" s="7">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="6">
-        <v>2860133353</v>
+        <v>2860124541</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="6" t="s">
         <v>44</v>
       </c>
       <c r="K26" s="21">
-        <v>0.27</v>
+        <v>10.06</v>
       </c>
       <c r="L26" s="21">
         <f t="shared" si="1"/>
@@ -1746,93 +1747,93 @@
       </c>
       <c r="M26" s="23"/>
     </row>
-    <row r="27" spans="1:13" s="26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="7">
-        <v>5077</v>
+        <v>5015</v>
       </c>
       <c r="B27" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="24" t="s">
-        <v>87</v>
+      <c r="F27" s="6">
+        <v>2860133353</v>
       </c>
       <c r="G27" s="24"/>
-      <c r="H27" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="H27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="6"/>
       <c r="J27" s="6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="K27" s="21">
-        <v>19.399999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="L27" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M27" s="25"/>
-    </row>
-    <row r="28" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="23"/>
+    </row>
+    <row r="28" spans="1:13" s="26" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="7">
-        <v>5080</v>
+        <v>5077</v>
       </c>
       <c r="B28" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="6" t="s">
-        <v>65</v>
+      <c r="F28" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="G28" s="24"/>
-      <c r="H28" s="6" t="s">
-        <v>66</v>
+      <c r="H28" s="24" t="s">
+        <v>88</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="K28" s="21">
-        <v>25.58</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="L28" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M28" s="23"/>
-    </row>
-    <row r="29" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M28" s="25"/>
+    </row>
+    <row r="29" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="7">
-        <v>5089</v>
+        <v>5080</v>
       </c>
       <c r="B29" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="24"/>
       <c r="E29" s="24"/>
       <c r="F29" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="G29" s="24"/>
       <c r="H29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I29" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="J29" s="6" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="K29" s="21">
-        <v>18.62</v>
+        <v>25.58</v>
       </c>
       <c r="L29" s="21">
         <f t="shared" si="1"/>
@@ -1840,31 +1841,29 @@
       </c>
       <c r="M29" s="23"/>
     </row>
-    <row r="30" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="7">
-        <v>5301</v>
+        <v>5089</v>
       </c>
       <c r="B30" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="24"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="24" t="s">
-        <v>17</v>
+      <c r="F30" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="G30" s="24"/>
       <c r="H30" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="I30" s="6"/>
       <c r="J30" s="6" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="K30" s="21">
-        <v>0.45</v>
+        <v>18.62</v>
       </c>
       <c r="L30" s="21">
         <f t="shared" si="1"/>
@@ -1872,29 +1871,31 @@
       </c>
       <c r="M30" s="23"/>
     </row>
-    <row r="31" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="7">
-        <v>5305</v>
+        <v>5301</v>
       </c>
       <c r="B31" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="6" t="s">
-        <v>105</v>
+      <c r="F31" s="24" t="s">
+        <v>17</v>
       </c>
       <c r="G31" s="24"/>
       <c r="H31" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="J31" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K31" s="21">
-        <v>9.1199999999999992</v>
+        <v>0.45</v>
       </c>
       <c r="L31" s="21">
         <f t="shared" si="1"/>
@@ -1902,9 +1903,9 @@
       </c>
       <c r="M31" s="23"/>
     </row>
-    <row r="32" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="7">
-        <v>5306</v>
+        <v>5305</v>
       </c>
       <c r="B32" s="7">
         <v>1</v>
@@ -1913,20 +1914,18 @@
       <c r="D32" s="24"/>
       <c r="E32" s="24"/>
       <c r="F32" s="6" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="G32" s="24"/>
       <c r="H32" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>69</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I32" s="6"/>
       <c r="J32" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K32" s="21">
-        <v>5.81</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="L32" s="21">
         <f t="shared" si="1"/>
@@ -1934,9 +1933,9 @@
       </c>
       <c r="M32" s="23"/>
     </row>
-    <row r="33" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="7">
-        <v>5307</v>
+        <v>5306</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
@@ -1945,18 +1944,20 @@
       <c r="D33" s="24"/>
       <c r="E33" s="24"/>
       <c r="F33" s="6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G33" s="24"/>
       <c r="H33" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I33" s="6"/>
+        <v>71</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="J33" s="6" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="K33" s="21">
-        <v>2.39</v>
+        <v>5.81</v>
       </c>
       <c r="L33" s="21">
         <f t="shared" si="1"/>
@@ -1964,9 +1965,9 @@
       </c>
       <c r="M33" s="23"/>
     </row>
-    <row r="34" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="7">
-        <v>5308</v>
+        <v>5307</v>
       </c>
       <c r="B34" s="7">
         <v>1</v>
@@ -1975,18 +1976,18 @@
       <c r="D34" s="24"/>
       <c r="E34" s="24"/>
       <c r="F34" s="6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="G34" s="24"/>
       <c r="H34" s="6" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="K34" s="21">
-        <v>9.15</v>
+        <v>2.39</v>
       </c>
       <c r="L34" s="21">
         <f t="shared" si="1"/>
@@ -1994,31 +1995,29 @@
       </c>
       <c r="M34" s="23"/>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="7">
-        <v>5310</v>
+        <v>5308</v>
       </c>
       <c r="B35" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="24"/>
       <c r="E35" s="24"/>
       <c r="F35" s="6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G35" s="24"/>
       <c r="H35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I35" s="6"/>
       <c r="J35" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K35" s="21">
-        <v>1.43</v>
+        <v>9.15</v>
       </c>
       <c r="L35" s="21">
         <f t="shared" si="1"/>
@@ -2026,31 +2025,31 @@
       </c>
       <c r="M35" s="23"/>
     </row>
-    <row r="36" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="7">
-        <v>5311</v>
+        <v>5310</v>
       </c>
       <c r="B36" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="24"/>
       <c r="E36" s="24"/>
       <c r="F36" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K36" s="21">
-        <v>0.43</v>
+        <v>1.43</v>
       </c>
       <c r="L36" s="21">
         <f t="shared" si="1"/>
@@ -2058,22 +2057,22 @@
       </c>
       <c r="M36" s="23"/>
     </row>
-    <row r="37" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="7">
-        <v>5313</v>
+        <v>5311</v>
       </c>
       <c r="B37" s="7">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="24"/>
       <c r="E37" s="24"/>
       <c r="F37" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G37" s="24"/>
       <c r="H37" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>22</v>
@@ -2082,7 +2081,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="21">
-        <v>2.66</v>
+        <v>0.43</v>
       </c>
       <c r="L37" s="21">
         <f t="shared" si="1"/>
@@ -2090,9 +2089,9 @@
       </c>
       <c r="M37" s="23"/>
     </row>
-    <row r="38" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="7">
-        <v>5315</v>
+        <v>5313</v>
       </c>
       <c r="B38" s="7">
         <v>1</v>
@@ -2100,21 +2099,21 @@
       <c r="C38" s="7"/>
       <c r="D38" s="24"/>
       <c r="E38" s="24"/>
-      <c r="F38" s="24" t="s">
-        <v>93</v>
+      <c r="F38" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="6" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="K38" s="21">
-        <v>12.2</v>
+        <v>2.66</v>
       </c>
       <c r="L38" s="21">
         <f t="shared" si="1"/>
@@ -2122,9 +2121,9 @@
       </c>
       <c r="M38" s="23"/>
     </row>
-    <row r="39" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="7">
-        <v>5318</v>
+        <v>5315</v>
       </c>
       <c r="B39" s="7">
         <v>1</v>
@@ -2132,21 +2131,21 @@
       <c r="C39" s="7"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
-      <c r="F39" s="6" t="s">
-        <v>28</v>
+      <c r="F39" s="24" t="s">
+        <v>93</v>
       </c>
       <c r="G39" s="24"/>
       <c r="H39" s="6" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="K39" s="21">
-        <v>1.2</v>
+        <v>12.2</v>
       </c>
       <c r="L39" s="21">
         <f t="shared" si="1"/>
@@ -2154,9 +2153,9 @@
       </c>
       <c r="M39" s="23"/>
     </row>
-    <row r="40" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="7">
-        <v>5321</v>
+        <v>5318</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
@@ -2165,20 +2164,20 @@
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G40" s="24"/>
       <c r="H40" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K40" s="21">
-        <v>1.05</v>
+        <v>1.2</v>
       </c>
       <c r="L40" s="21">
         <f t="shared" si="1"/>
@@ -2186,22 +2185,22 @@
       </c>
       <c r="M40" s="23"/>
     </row>
-    <row r="41" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="7">
-        <v>5323</v>
+        <v>5321</v>
       </c>
       <c r="B41" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="24"/>
       <c r="E41" s="24"/>
       <c r="F41" s="6" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="G41" s="24"/>
       <c r="H41" s="6" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>13</v>
@@ -2210,7 +2209,7 @@
         <v>14</v>
       </c>
       <c r="K41" s="21">
-        <v>1.4</v>
+        <v>1.05</v>
       </c>
       <c r="L41" s="21">
         <f t="shared" si="1"/>
@@ -2218,22 +2217,22 @@
       </c>
       <c r="M41" s="23"/>
     </row>
-    <row r="42" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="7">
-        <v>5324</v>
+        <v>5323</v>
       </c>
       <c r="B42" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="24"/>
       <c r="E42" s="24"/>
       <c r="F42" s="6" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="G42" s="24"/>
       <c r="H42" s="6" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>13</v>
@@ -2242,69 +2241,71 @@
         <v>14</v>
       </c>
       <c r="K42" s="21">
-        <v>0.95</v>
+        <v>1.4</v>
       </c>
       <c r="L42" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M42" s="28"/>
-    </row>
-    <row r="43" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M42" s="23"/>
+    </row>
+    <row r="43" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="7">
-        <v>5327</v>
+        <v>5324</v>
       </c>
       <c r="B43" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="24"/>
       <c r="E43" s="24"/>
-      <c r="F43" s="24">
-        <v>108408</v>
+      <c r="F43" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="G43" s="24"/>
       <c r="H43" s="6" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>124</v>
+        <v>14</v>
       </c>
       <c r="K43" s="21">
-        <v>4.42</v>
+        <v>0.95</v>
       </c>
       <c r="L43" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M43" s="23"/>
-    </row>
-    <row r="44" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M43" s="28"/>
+    </row>
+    <row r="44" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="7">
-        <v>5328</v>
+        <v>5327</v>
       </c>
       <c r="B44" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="24"/>
       <c r="E44" s="24"/>
-      <c r="F44" s="6">
-        <v>2860105462</v>
+      <c r="F44" s="24">
+        <v>108408</v>
       </c>
       <c r="G44" s="24"/>
       <c r="H44" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I44" s="6"/>
+        <v>38</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="J44" s="6" t="s">
-        <v>44</v>
+        <v>124</v>
       </c>
       <c r="K44" s="21">
-        <v>2.97</v>
+        <v>4.42</v>
       </c>
       <c r="L44" s="21">
         <f t="shared" si="1"/>
@@ -2312,31 +2313,29 @@
       </c>
       <c r="M44" s="23"/>
     </row>
-    <row r="45" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="7">
-        <v>5336</v>
+        <v>5328</v>
       </c>
       <c r="B45" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="24"/>
       <c r="E45" s="24"/>
-      <c r="F45" s="24">
-        <v>120760</v>
+      <c r="F45" s="6">
+        <v>2860105462</v>
       </c>
       <c r="G45" s="24"/>
       <c r="H45" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I45" s="24" t="s">
-        <v>34</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="I45" s="6"/>
       <c r="J45" s="6" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="K45" s="21">
-        <v>2.4700000000000002</v>
+        <v>2.97</v>
       </c>
       <c r="L45" s="21">
         <f t="shared" si="1"/>
@@ -2344,9 +2343,9 @@
       </c>
       <c r="M45" s="23"/>
     </row>
-    <row r="46" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="7">
-        <v>5337</v>
+        <v>5336</v>
       </c>
       <c r="B46" s="7">
         <v>1</v>
@@ -2355,20 +2354,20 @@
       <c r="D46" s="24"/>
       <c r="E46" s="24"/>
       <c r="F46" s="24">
-        <v>120771</v>
+        <v>120760</v>
       </c>
       <c r="G46" s="24"/>
       <c r="H46" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I46" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="24" t="s">
         <v>34</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>124</v>
       </c>
       <c r="K46" s="21">
-        <v>3.19</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="L46" s="21">
         <f t="shared" si="1"/>
@@ -2376,31 +2375,31 @@
       </c>
       <c r="M46" s="23"/>
     </row>
-    <row r="47" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="7">
-        <v>5338</v>
+        <v>5337</v>
       </c>
       <c r="B47" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="24"/>
       <c r="E47" s="24"/>
-      <c r="F47" s="6" t="s">
-        <v>52</v>
+      <c r="F47" s="24">
+        <v>120771</v>
       </c>
       <c r="G47" s="24"/>
-      <c r="H47" s="24" t="s">
-        <v>53</v>
+      <c r="H47" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="K47" s="21">
-        <v>6.9</v>
+        <v>3.19</v>
       </c>
       <c r="L47" s="21">
         <f t="shared" si="1"/>
@@ -2408,31 +2407,31 @@
       </c>
       <c r="M47" s="23"/>
     </row>
-    <row r="48" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="7">
-        <v>5339</v>
+        <v>5338</v>
       </c>
       <c r="B48" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="24"/>
       <c r="E48" s="24"/>
       <c r="F48" s="6" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="G48" s="24"/>
-      <c r="H48" s="6" t="s">
-        <v>42</v>
+      <c r="H48" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="K48" s="21">
-        <v>1.06</v>
+        <v>6.9</v>
       </c>
       <c r="L48" s="21">
         <f t="shared" si="1"/>
@@ -2440,9 +2439,9 @@
       </c>
       <c r="M48" s="23"/>
     </row>
-    <row r="49" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="7">
-        <v>5340</v>
+        <v>5339</v>
       </c>
       <c r="B49" s="7">
         <v>1</v>
@@ -2451,11 +2450,11 @@
       <c r="D49" s="24"/>
       <c r="E49" s="24"/>
       <c r="F49" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G49" s="24"/>
       <c r="H49" s="6" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>43</v>
@@ -2472,9 +2471,9 @@
       </c>
       <c r="M49" s="23"/>
     </row>
-    <row r="50" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="7">
-        <v>5341</v>
+        <v>5340</v>
       </c>
       <c r="B50" s="7">
         <v>1</v>
@@ -2483,20 +2482,20 @@
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
       <c r="F50" s="6" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="G50" s="24"/>
       <c r="H50" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="K50" s="21">
-        <v>14.7</v>
+        <v>1.06</v>
       </c>
       <c r="L50" s="21">
         <f t="shared" si="1"/>
@@ -2504,9 +2503,9 @@
       </c>
       <c r="M50" s="23"/>
     </row>
-    <row r="51" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="7">
-        <v>5342</v>
+        <v>5341</v>
       </c>
       <c r="B51" s="7">
         <v>1</v>
@@ -2514,23 +2513,21 @@
       <c r="C51" s="7"/>
       <c r="D51" s="24"/>
       <c r="E51" s="24"/>
-      <c r="F51" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>57</v>
-      </c>
+      <c r="F51" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G51" s="24"/>
       <c r="H51" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="K51" s="21">
-        <v>1.17</v>
+        <v>14.7</v>
       </c>
       <c r="L51" s="21">
         <f t="shared" si="1"/>
@@ -2538,9 +2535,9 @@
       </c>
       <c r="M51" s="23"/>
     </row>
-    <row r="52" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="7">
-        <v>5343</v>
+        <v>5342</v>
       </c>
       <c r="B52" s="7">
         <v>1</v>
@@ -2549,22 +2546,22 @@
       <c r="D52" s="24"/>
       <c r="E52" s="24"/>
       <c r="F52" s="24" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>58</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K52" s="21">
-        <v>1.85</v>
+        <v>1.17</v>
       </c>
       <c r="L52" s="21">
         <f t="shared" si="1"/>
@@ -2572,32 +2569,33 @@
       </c>
       <c r="M52" s="23"/>
     </row>
-    <row r="53" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="7">
-        <v>5185</v>
+        <v>5343</v>
       </c>
       <c r="B53" s="7">
-        <v>2</v>
-      </c>
-      <c r="C53" s="7">
-        <f>SUM(B53*D49)</f>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C53" s="7"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
-      <c r="F53" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G53" s="24"/>
-      <c r="H53" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="I53" s="6"/>
+      <c r="F53" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="J53" s="6" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="K53" s="21">
-        <v>0.66</v>
+        <v>1.85</v>
       </c>
       <c r="L53" s="21">
         <f t="shared" si="1"/>
@@ -2605,47 +2603,80 @@
       </c>
       <c r="M53" s="23"/>
     </row>
-    <row r="54" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="10" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="7">
-        <v>5320</v>
+        <v>5185</v>
       </c>
       <c r="B54" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54" s="7">
-        <f>SUM(B54*D48)</f>
+        <f>SUM(B54*D50)</f>
         <v>0</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24"/>
-      <c r="F54" s="6" t="s">
+      <c r="F54" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G54" s="24"/>
+      <c r="H54" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K54" s="21">
+        <v>0.66</v>
+      </c>
+      <c r="L54" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="23"/>
+    </row>
+    <row r="55" spans="1:13" s="29" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="7">
+        <v>5320</v>
+      </c>
+      <c r="B55" s="7">
+        <v>1</v>
+      </c>
+      <c r="C55" s="7">
+        <f>SUM(B55*D49)</f>
+        <v>0</v>
+      </c>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24"/>
+      <c r="F55" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G54" s="24"/>
-      <c r="H54" s="6" t="s">
+      <c r="G55" s="24"/>
+      <c r="H55" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I54" s="6" t="s">
+      <c r="I55" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J54" s="6" t="s">
+      <c r="J55" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K54" s="21">
+      <c r="K55" s="21">
         <v>2.4300000000000002</v>
       </c>
-      <c r="L54" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M54" s="28"/>
+      <c r="L55" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="28"/>
     </row>
   </sheetData>
   <sortState ref="A9:K58">
     <sortCondition ref="A58"/>
   </sortState>
   <mergeCells count="7">
-    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="H2:I2"/>

</xml_diff>